<commit_message>
Added units from new unit lists received 21 Sep
</commit_message>
<xml_diff>
--- a/app/static/unit data files/Unit list 12520 Master of Translation Studies.xlsx
+++ b/app/static/unit data files/Unit list 12520 Master of Translation Studies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/21627616_student_uwa_edu_au/Documents/Year 2 Semester 2/CITS5206 Information Technology Capstone Project/CAIDi system/Files used - to be played with/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa.sharepoint.com/teams/CITS5206SEM-22022-StudyPlannerTeam1/Shared Documents/Study Planner Team 1/CAIDi system/FILES USED IN WEB APPLICATION/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="5" documentId="11_24A1611706D4B35FFBB70DF9BA47942B44B867EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{895E13A6-722F-4B74-996D-7AB8D10B7113}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="8002" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31770" yWindow="285" windowWidth="21525" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit list" sheetId="1" r:id="rId1"/>
@@ -1606,7 +1606,7 @@
   <dimension ref="A1:AD41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5083,15 +5083,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A49CD37CF5DEE4094795E34A11BD8BC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="72135e89fd6a0103cf3b8bcfa7f615d2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9f6f0188-c21b-4c3f-be91-a9139ad3a050" xmlns:ns3="a90a73a0-65dd-424f-b0e8-24cf385fc12c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a1860a4e810b4a51a4f98638da7b5da" ns2:_="" ns3:_="">
     <xsd:import namespace="9f6f0188-c21b-4c3f-be91-a9139ad3a050"/>
@@ -5296,15 +5287,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{116BB1E0-122A-4C0A-A0E7-6E23CD790487}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD81D00C-EBE3-4769-8A20-205DD992EDC0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5321,4 +5313,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{116BB1E0-122A-4C0A-A0E7-6E23CD790487}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>